<commit_message>
Update ABA_Questionnaire Recommendation Engine Improvement.xlsx
</commit_message>
<xml_diff>
--- a/Sprint 3/ABA_Questionnaire Recommendation Engine Improvement.xlsx
+++ b/Sprint 3/ABA_Questionnaire Recommendation Engine Improvement.xlsx
@@ -5,17 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stda/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stda/Documents/GitHub/01_TEAM/Sprint 3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AF5AB8E4-BE78-374A-8213-D1D55888D4E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8B4FF29-ACAA-BE43-9986-052D48917E2A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{688622EC-6FCF-BD4D-8C83-4413250CEE5F}"/>
+    <workbookView xWindow="560" yWindow="1300" windowWidth="32420" windowHeight="18080" xr2:uid="{688622EC-6FCF-BD4D-8C83-4413250CEE5F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Questionnaire Results" sheetId="3" r:id="rId1"/>
+    <sheet name="Questionnaire Background" sheetId="2" r:id="rId2"/>
+    <sheet name="Utilities" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="60">
   <si>
     <t>1 – How would you categorize your partner's job?</t>
   </si>
@@ -126,13 +128,100 @@
   </si>
   <si>
     <t>Freetext Answer</t>
+  </si>
+  <si>
+    <t>Participant</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Tipp suggested by recommendation system</t>
+  </si>
+  <si>
+    <t>Match</t>
+  </si>
+  <si>
+    <t>Aline</t>
+  </si>
+  <si>
+    <t>Answers</t>
+  </si>
+  <si>
+    <t>Tipps</t>
+  </si>
+  <si>
+    <t>Tipp A</t>
+  </si>
+  <si>
+    <t>Tipp B</t>
+  </si>
+  <si>
+    <t>Tipp C</t>
+  </si>
+  <si>
+    <t>Participants</t>
+  </si>
+  <si>
+    <t>Hits</t>
+  </si>
+  <si>
+    <t>Accuracy</t>
+  </si>
+  <si>
+    <t>Results</t>
+  </si>
+  <si>
+    <t>Peter</t>
+  </si>
+  <si>
+    <t>Simon</t>
+  </si>
+  <si>
+    <t>Caroline</t>
+  </si>
+  <si>
+    <t>Leo</t>
+  </si>
+  <si>
+    <t>Patricia</t>
+  </si>
+  <si>
+    <t>Severin</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>Playing a board game</t>
+  </si>
+  <si>
+    <t>Going for a ride with a car</t>
+  </si>
+  <si>
+    <t>Going to a music concert</t>
+  </si>
+  <si>
+    <t>Go for a walk</t>
+  </si>
+  <si>
+    <t>Read a book together</t>
+  </si>
+  <si>
+    <t>cycling tour</t>
+  </si>
+  <si>
+    <t>Playing a video game together</t>
+  </si>
+  <si>
+    <t>Watching a nice movie at home</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -148,8 +237,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -180,6 +276,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="20">
     <border>
@@ -451,15 +559,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -468,6 +574,75 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -475,66 +650,18 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Per cent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -845,11 +972,461 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57634428-D074-0749-B81B-6D17A835EEEE}">
+  <dimension ref="A3:M29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="3.83203125" style="1" customWidth="1"/>
+    <col min="3" max="6" width="29.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="29.6640625" customWidth="1"/>
+    <col min="8" max="8" width="3.5" customWidth="1"/>
+    <col min="9" max="9" width="22.83203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.33203125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="3.5" customWidth="1"/>
+    <col min="12" max="12" width="13.33203125" customWidth="1"/>
+    <col min="13" max="13" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:13" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" s="25"/>
+      <c r="I3" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="L3" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="M3" s="30"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J4" s="1">
+        <f>IF(I4=F4,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="L4" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="M4" s="1">
+        <f>COUNT(J4:J50)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J5" s="1">
+        <f>IF(F5="","",IF(I5=F5,1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="L5" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="M5" s="1">
+        <f>SUM(J4:J42)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J6" s="1">
+        <f t="shared" ref="J6:J29" si="0">IF(F6="","",IF(I6=F6,1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="L6" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="M6" s="28">
+        <f>M5/M4</f>
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J7" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J8" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J9" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J10" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J11" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="J12" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="J13" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="J14" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="J15" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="J16" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J17" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J18" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J19" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J20" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J21" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J22" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J23" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J24" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J25" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J26" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J27" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J28" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J29" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="L3:M3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C64E976D-E26F-7847-96E2-E1549684219D}">
+          <x14:formula1>
+            <xm:f>Utilities!$B$4:$B$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>C4:E26</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{77507ED1-5362-9148-AA03-BD82B9CA8ABB}">
+          <x14:formula1>
+            <xm:f>Utilities!$C$4:$C$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>F4:F24 I4:I30</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA81D99E-D4F6-A540-B32E-E2A087BF1BA2}">
   <dimension ref="B1:I29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="160" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView showGridLines="0" topLeftCell="A5" zoomScale="160" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -864,268 +1441,268 @@
   <sheetData>
     <row r="1" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="16">
+      <c r="D2" s="13">
         <v>1</v>
       </c>
-      <c r="E2" s="17">
+      <c r="E2" s="14">
         <v>2</v>
       </c>
-      <c r="F2" s="18">
+      <c r="F2" s="15">
         <v>3</v>
       </c>
-      <c r="G2" s="22" t="s">
+      <c r="G2" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="19" t="s">
+      <c r="F3" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="23" t="s">
+      <c r="G3" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="I3" s="6" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="20" t="s">
+      <c r="F4" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="24" t="s">
+      <c r="G4" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="I4" s="9" t="s">
+      <c r="I4" s="6" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="5" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" s="24" t="s">
+      <c r="F5" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="I5" s="10" t="s">
+      <c r="I5" s="7" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="6" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="20" t="s">
+      <c r="F6" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="24" t="s">
+      <c r="G6" s="21" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="7" spans="2:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="G7" s="24" t="s">
+      <c r="E7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="I7" s="7" t="s">
+      <c r="I7" s="31" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="20" t="s">
+      <c r="E8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="24" t="s">
+      <c r="G8" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="8"/>
+      <c r="I8" s="32"/>
     </row>
     <row r="9" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="3" t="s">
+      <c r="D9" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="G9" s="24" t="s">
+      <c r="F9" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="I9" s="10" t="s">
+      <c r="I9" s="7" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="10" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="3" t="s">
+      <c r="D10" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="20" t="s">
+      <c r="F10" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="24" t="s">
+      <c r="G10" s="21" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="11" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D11" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F11" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="G11" s="24" t="s">
+      <c r="D11" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="21" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F12" s="20" t="s">
+      <c r="D12" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="G12" s="24" t="s">
+      <c r="G12" s="21" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="13" spans="2:9" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="8"/>
-      <c r="D13" s="11" t="s">
+      <c r="B13" s="32"/>
+      <c r="D13" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F13" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="G13" s="24" t="s">
+      <c r="F13" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="21" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="E14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F14" s="20" t="s">
+      <c r="F14" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="G14" s="24" t="s">
+      <c r="G14" s="21" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="D15" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F15" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="G15" s="24" t="s">
+      <c r="E15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="21" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="16" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E16" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="F16" s="21" t="s">
+      <c r="E16" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="G16" s="25" t="s">
+      <c r="G16" s="22" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1135,26 +1712,26 @@
       <c r="F17" s="1"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B18" s="26" t="s">
+      <c r="B18" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
+      <c r="E18" s="35"/>
+      <c r="F18" s="35"/>
+      <c r="G18" s="35"/>
     </row>
     <row r="19" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
+      <c r="E19" s="35"/>
+      <c r="F19" s="35"/>
+      <c r="G19" s="35"/>
     </row>
     <row r="20" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D20" s="1"/>
@@ -1163,7 +1740,7 @@
       <c r="G20" s="1"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B21" s="26" t="s">
+      <c r="B21" s="23" t="s">
         <v>17</v>
       </c>
       <c r="D21" s="1"/>
@@ -1171,7 +1748,7 @@
       <c r="F21" s="1"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B22" s="27" t="s">
+      <c r="B22" s="33" t="s">
         <v>19</v>
       </c>
       <c r="D22" s="1"/>
@@ -1179,13 +1756,13 @@
       <c r="F22" s="1"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B23" s="27"/>
+      <c r="B23" s="33"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
     </row>
     <row r="24" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="28"/>
+      <c r="B24" s="34"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
@@ -1196,7 +1773,7 @@
       <c r="F25" s="1"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B26" s="26" t="s">
+      <c r="B26" s="23" t="s">
         <v>20</v>
       </c>
       <c r="D26" s="1"/>
@@ -1204,7 +1781,7 @@
       <c r="F26" s="1"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B27" s="27" t="s">
+      <c r="B27" s="33" t="s">
         <v>22</v>
       </c>
       <c r="D27" s="1"/>
@@ -1213,7 +1790,7 @@
       <c r="G27" s="1"/>
     </row>
     <row r="28" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="28"/>
+      <c r="B28" s="34"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
@@ -1227,13 +1804,60 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="I7:I8"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="B22:B24"/>
     <mergeCell ref="B27:B28"/>
     <mergeCell ref="D18:G18"/>
     <mergeCell ref="D19:G19"/>
-    <mergeCell ref="I7:I8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16CC4905-2003-354D-A3A6-D42A68536B7F}">
+  <dimension ref="B3:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B3" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added validation results spint 3
</commit_message>
<xml_diff>
--- a/Sprint 3/ABA_Questionnaire Recommendation Engine Improvement.xlsx
+++ b/Sprint 3/ABA_Questionnaire Recommendation Engine Improvement.xlsx
@@ -5,18 +5,25 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/TheGod/Dropbox/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stda/Documents/GitHub/01_TEAM/Sprint 3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4EFD6A89-75B3-F649-99C7-C7F2C30A1942}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB784178-47CE-3940-AB39-404C9D0DEE71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="1300" windowWidth="32420" windowHeight="18080" xr2:uid="{688622EC-6FCF-BD4D-8C83-4413250CEE5F}"/>
+    <workbookView xWindow="920" yWindow="1300" windowWidth="32420" windowHeight="18080" activeTab="2" xr2:uid="{688622EC-6FCF-BD4D-8C83-4413250CEE5F}"/>
   </bookViews>
   <sheets>
     <sheet name="Questionnaire Results" sheetId="3" r:id="rId1"/>
     <sheet name="Questionnaire Background" sheetId="2" r:id="rId2"/>
     <sheet name="Utilities" sheetId="4" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Questionnaire Results'!$A$3:$J$27</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Utilities!$B$29:$B$35</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Utilities!$C$29:$C$35</definedName>
+    <definedName name="_xlchart.v2.0" hidden="1">Utilities!$B$29:$B$35</definedName>
+    <definedName name="_xlchart.v2.1" hidden="1">Utilities!$C$29:$C$35</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +32,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="79">
   <si>
     <t>1 – How would you categorize your partner's job?</t>
   </si>
@@ -191,9 +200,6 @@
     <t>David</t>
   </si>
   <si>
-    <t>Playing a board game</t>
-  </si>
-  <si>
     <t>Going to a music concert</t>
   </si>
   <si>
@@ -227,9 +233,6 @@
     <t>Hong</t>
   </si>
   <si>
-    <t>Going to a playhall to play bowling</t>
-  </si>
-  <si>
     <t>Kemal</t>
   </si>
   <si>
@@ -258,6 +261,24 @@
   </si>
   <si>
     <t>Shopping or going to a museum</t>
+  </si>
+  <si>
+    <t>Indoor activity like bowling</t>
+  </si>
+  <si>
+    <t>Dino</t>
+  </si>
+  <si>
+    <t>Kevin</t>
+  </si>
+  <si>
+    <t>Sarah</t>
+  </si>
+  <si>
+    <t>Jana</t>
+  </si>
+  <si>
+    <t>Adam</t>
   </si>
 </sst>
 </file>
@@ -606,7 +627,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -701,10 +722,14 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Prozent" xfId="1" builtinId="5"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Per cent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -719,8 +744,2139 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="75000"/>
+                  <a:lumOff val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:pattFill prst="pct75">
+                <a:fgClr>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
+                  </a:schemeClr>
+                </a:fgClr>
+                <a:bgClr>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:bgClr>
+              </a:pattFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="de-DE"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="50000"/>
+                      <a:lumOff val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Utilities!$B$15:$B$17</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Tipp B</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Tipp A</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Tipp C</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Utilities!$C$15:$C$17</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.64</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.27</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.09</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-019C-3643-BF42-18DB7DAB39E6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="ctr"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="39000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="75000"/>
+                  <a:lumOff val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="lt1"/>
+        </a:gs>
+        <a:gs pos="39000">
+          <a:schemeClr val="lt1"/>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="lt1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="25000"/>
+          <a:lumOff val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="75000"/>
+                  <a:lumOff val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:pattFill prst="pct75">
+                <a:fgClr>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
+                  </a:schemeClr>
+                </a:fgClr>
+                <a:bgClr>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:bgClr>
+              </a:pattFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="de-DE"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="50000"/>
+                      <a:lumOff val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Utilities!$B$29:$B$35</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Outdoor activity like hiking</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Shopping</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Going to a music concert</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Watching a nice movie at home</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Go for a walk</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Indoor activity like bowling</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Having dinner together</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Utilities!$C$29:$C$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7D98-B240-B49D-04A21952A148}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="ctr"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.62539567469871449"/>
+          <c:y val="0.20295969508013539"/>
+          <c:w val="0.35813431530904721"/>
+          <c:h val="0.72991815534255489"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="39000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="75000"/>
+                  <a:lumOff val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="lt1"/>
+        </a:gs>
+        <a:gs pos="39000">
+          <a:schemeClr val="lt1"/>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="lt1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="25000"/>
+          <a:lumOff val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="253">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="all" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+          <a:gs pos="39000">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="lt1">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="pct75">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+    <cs:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="pct75">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+    <cs:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="20000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="20000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="31750" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="95000"/>
+                <a:lumOff val="5000"/>
+                <a:alpha val="42000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1">
+                <a:lumMod val="75000"/>
+                <a:alpha val="36000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="95000"/>
+                <a:lumOff val="5000"/>
+                <a:alpha val="42000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1">
+                <a:lumMod val="75000"/>
+                <a:alpha val="36000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="95000"/>
+          <a:alpha val="39000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="31750" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1800" b="1" kern="1200" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="253">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="all" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+          <a:gs pos="39000">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="lt1">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="pct75">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+    <cs:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="pct75">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+    <cs:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="20000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="20000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="31750" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="95000"/>
+                <a:lumOff val="5000"/>
+                <a:alpha val="42000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1">
+                <a:lumMod val="75000"/>
+                <a:alpha val="36000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="95000"/>
+                <a:lumOff val="5000"/>
+                <a:alpha val="42000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1">
+                <a:lumMod val="75000"/>
+                <a:alpha val="36000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="95000"/>
+          <a:alpha val="39000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="31750" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1800" b="1" kern="1200" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>169877</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>132302</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>73594</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>135699</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9163D9DA-8560-2241-A27C-21015150824E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>318081</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>160556</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>104099</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>11653</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{35BCD053-D8A9-2D40-9DCA-97ED38765C46}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1018,8 +3174,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57634428-D074-0749-B81B-6D17A835EEEE}">
   <dimension ref="A3:M29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView topLeftCell="C1" zoomScale="125" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4:G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1089,7 +3245,7 @@
         <v>39</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>38</v>
@@ -1103,7 +3259,7 @@
       </c>
       <c r="M4" s="1">
         <f>COUNT(J4:J50)</f>
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
@@ -1126,7 +3282,7 @@
         <v>38</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>39</v>
@@ -1140,7 +3296,7 @@
       </c>
       <c r="M5" s="1">
         <f>SUM(J4:J42)</f>
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
@@ -1163,7 +3319,7 @@
         <v>39</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>39</v>
@@ -1177,7 +3333,7 @@
       </c>
       <c r="M6" s="28">
         <f>M5/M4</f>
-        <v>0.52631578947368418</v>
+        <v>0.54166666666666663</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
@@ -1200,7 +3356,7 @@
         <v>39</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>39</v>
@@ -1230,7 +3386,7 @@
         <v>38</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>38</v>
@@ -1260,7 +3416,7 @@
         <v>39</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>39</v>
@@ -1287,10 +3443,10 @@
         <v>13</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>40</v>
@@ -1320,7 +3476,7 @@
         <v>38</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>38</v>
@@ -1335,7 +3491,7 @@
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>13</v>
@@ -1350,7 +3506,7 @@
         <v>38</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>38</v>
@@ -1365,7 +3521,7 @@
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>13</v>
@@ -1380,7 +3536,7 @@
         <v>38</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>39</v>
@@ -1395,7 +3551,7 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>13</v>
@@ -1410,7 +3566,7 @@
         <v>39</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>39</v>
@@ -1425,7 +3581,7 @@
         <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>13</v>
@@ -1440,7 +3596,7 @@
         <v>39</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>38</v>
@@ -1455,7 +3611,7 @@
         <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>13</v>
@@ -1470,7 +3626,7 @@
         <v>40</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>40</v>
@@ -1485,7 +3641,7 @@
         <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>12</v>
@@ -1500,7 +3656,7 @@
         <v>38</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>40</v>
@@ -1515,7 +3671,7 @@
         <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>13</v>
@@ -1542,7 +3698,7 @@
         <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>13</v>
@@ -1557,7 +3713,7 @@
         <v>39</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>38</v>
@@ -1572,7 +3728,7 @@
         <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>13</v>
@@ -1587,7 +3743,7 @@
         <v>40</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>39</v>
@@ -1602,7 +3758,7 @@
         <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>12</v>
@@ -1629,7 +3785,7 @@
         <v>19</v>
       </c>
       <c r="B22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>13</v>
@@ -1644,7 +3800,7 @@
         <v>40</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>40</v>
@@ -1655,33 +3811,153 @@
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J23" s="1" t="str">
+      <c r="A23" s="1">
+        <v>20</v>
+      </c>
+      <c r="B23" t="s">
+        <v>74</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J23" s="1">
         <f t="shared" si="0"/>
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J24" s="1" t="str">
+      <c r="A24" s="1">
+        <v>21</v>
+      </c>
+      <c r="B24" t="s">
+        <v>75</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J24" s="1">
         <f t="shared" si="0"/>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J25" s="1" t="str">
+      <c r="A25" s="1">
+        <v>22</v>
+      </c>
+      <c r="B25" t="s">
+        <v>76</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J25" s="1">
         <f t="shared" si="0"/>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J26" s="1" t="str">
+      <c r="A26" s="1">
+        <v>23</v>
+      </c>
+      <c r="B26" t="s">
+        <v>77</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J26" s="1">
         <f t="shared" si="0"/>
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J27" s="1" t="str">
+      <c r="A27" s="1">
+        <v>24</v>
+      </c>
+      <c r="B27" t="s">
+        <v>78</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J27" s="1">
         <f t="shared" si="0"/>
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
@@ -1697,6 +3973,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A3:J27" xr:uid="{F606619E-30F0-B040-BCC8-7545B8F246EB}"/>
   <mergeCells count="1">
     <mergeCell ref="L3:M3"/>
   </mergeCells>
@@ -1708,13 +3985,13 @@
           <x14:formula1>
             <xm:f>Utilities!$B$4:$B$6</xm:f>
           </x14:formula1>
-          <xm:sqref>C4:E26</xm:sqref>
+          <xm:sqref>C4:E27</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{77507ED1-5362-9148-AA03-BD82B9CA8ABB}">
           <x14:formula1>
             <xm:f>Utilities!$C$4:$C$6</xm:f>
           </x14:formula1>
-          <xm:sqref>F4:F24 I4:I30</xm:sqref>
+          <xm:sqref>F4:F27 I4:I30</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2118,13 +4395,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16CC4905-2003-354D-A3A6-D42A68536B7F}">
-  <dimension ref="B3:C6"/>
+  <dimension ref="B3:C46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="C27" zoomScale="244" workbookViewId="0">
+      <selection activeCell="K36" sqref="K36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="29.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="3" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B3" s="24" t="s">
@@ -2158,7 +4438,121 @@
         <v>40</v>
       </c>
     </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="36">
+        <v>0.64</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="36">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="36">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B29" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="C29">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B30" s="37" t="s">
+        <v>58</v>
+      </c>
+      <c r="C30">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B31" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="C31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B32" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="C32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B33" s="37" t="s">
+        <v>53</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B34" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="C34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B35" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B36" s="37"/>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B37" s="37"/>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B38" s="37"/>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B39" s="37"/>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B40" s="37"/>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B41" s="37"/>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B42" s="37"/>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B43" s="37"/>
+    </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B44" s="37"/>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B45" s="37"/>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B46" s="37"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>